<commit_message>
Find minimum in rotated sorted array
</commit_message>
<xml_diff>
--- a/DSA_sheet.xlsx
+++ b/DSA_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PKIRANMU\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10F4FBF-415A-4B95-A69C-4E2A0A350BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF134FA5-2E04-400F-934F-5797C8CC1629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,10 +24,10 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="701">
   <si>
     <t>DSA by Shradha Ma'am</t>
   </si>
@@ -2741,8 +2741,8 @@
   </sheetPr>
   <dimension ref="A1:AC914"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="105" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="105" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3464,7 +3464,9 @@
         <v>39</v>
       </c>
       <c r="C20" s="11"/>
-      <c r="D20" s="41"/>
+      <c r="D20" s="40" t="s">
+        <v>700</v>
+      </c>
       <c r="E20" s="12" t="s">
         <v>40</v>
       </c>
@@ -33209,21 +33211,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{B3F80A84-1911-4657-9764-20E00EF707E3}"/>
+      <autoFilter ref="A11:C37" xr:uid="{5FCD45F0-2EDE-439B-B88C-B06DE01B17D4}"/>
+    </customSheetView>
+    <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A11:D37" xr:uid="{24B2E198-F00C-4D39-9AD5-BCE865667DCD}"/>
     </customSheetView>
     <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{EB86E71A-1F82-4E99-BB9C-DE23D7B1593A}"/>
+      <autoFilter ref="A11:D37" xr:uid="{FA53436A-13C9-43D6-8776-5B5D70E16714}"/>
     </customSheetView>
-    <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{8E7B8E09-DE0D-467D-A99F-53183D2743E8}"/>
-    </customSheetView>
-    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{D654521A-AA6B-4CEC-B2D7-EC5462C09FEF}"/>
+      <autoFilter ref="A293:C332" xr:uid="{E078AE93-05A3-489C-A045-BA729FD90156}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Container with Max Water
</commit_message>
<xml_diff>
--- a/DSA_sheet.xlsx
+++ b/DSA_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PKIRANMU\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4029331B-6AD6-48CE-8339-9B83D970D395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47112839-C0D1-4CBD-A065-116460E6C602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,10 +24,10 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="701">
   <si>
     <t>DSA by Shradha Ma'am</t>
   </si>
@@ -2739,7 +2739,7 @@
   <dimension ref="A1:AC914"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" zoomScale="105" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3539,7 +3539,9 @@
         <v>43</v>
       </c>
       <c r="C22" s="11"/>
-      <c r="D22" s="41"/>
+      <c r="D22" s="40" t="s">
+        <v>700</v>
+      </c>
       <c r="E22" s="12" t="s">
         <v>40</v>
       </c>
@@ -3576,7 +3578,9 @@
         <v>44</v>
       </c>
       <c r="C23" s="11"/>
-      <c r="D23" s="41"/>
+      <c r="D23" s="40" t="s">
+        <v>700</v>
+      </c>
       <c r="E23" s="12" t="s">
         <v>45</v>
       </c>
@@ -33210,21 +33214,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{47761B09-D8BA-4891-89BD-016B644F4602}"/>
+      <autoFilter ref="A11:C37" xr:uid="{67288A8F-AC6E-4FFD-8B5E-5E3D5E5A65CA}"/>
+    </customSheetView>
+    <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A11:D37" xr:uid="{42B8C2AE-708A-466A-B2B1-1B36D2FFAB54}"/>
     </customSheetView>
     <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{F57A0DE6-560A-4F65-97D4-B0A927210257}"/>
+      <autoFilter ref="A11:D37" xr:uid="{7D73781B-1106-4C16-902F-9A128749BD94}"/>
     </customSheetView>
-    <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{DEE7166D-69F5-4889-8C19-3B4AB44A8C6C}"/>
-    </customSheetView>
-    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{B8D18A8B-099B-4A64-B0F2-CB9F62BCE241}"/>
+      <autoFilter ref="A293:C332" xr:uid="{21FA3932-3FA2-43EF-8C6F-C413933049C5}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Minimum of merge operations to make an array Palindrome
</commit_message>
<xml_diff>
--- a/DSA_sheet.xlsx
+++ b/DSA_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PKIRANMU\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA36C29-39F5-406C-B613-32531176E4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF14A604-BFE0-4D59-AED1-31622B98B582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,10 +24,10 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1256" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="701">
   <si>
     <t>DSA by Shradha Ma'am</t>
   </si>
@@ -3736,7 +3736,9 @@
         <v>52</v>
       </c>
       <c r="C27" s="11"/>
-      <c r="D27" s="41"/>
+      <c r="D27" s="40" t="s">
+        <v>700</v>
+      </c>
       <c r="E27" s="12" t="s">
         <v>53</v>
       </c>
@@ -33219,21 +33221,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{9BB792A4-4218-497D-936F-7F5C1E416285}"/>
+      <autoFilter ref="A11:C37" xr:uid="{0ACB2A45-7D75-4140-937B-E1EEB2CA3B90}"/>
+    </customSheetView>
+    <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A11:D37" xr:uid="{5B33EC87-A986-47DA-AEE2-0FD74F8ADB55}"/>
     </customSheetView>
     <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{FD45CAC0-DAAE-46DD-B681-8031936F18C1}"/>
+      <autoFilter ref="A11:D37" xr:uid="{5D3BF9DF-E222-4578-A829-977AD89160C5}"/>
     </customSheetView>
-    <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{C3BA4ACB-291B-4DED-A6C5-EB05B33FA12F}"/>
-    </customSheetView>
-    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{A3C53268-092D-4508-91DE-03D0C51F0638}"/>
+      <autoFilter ref="A293:C332" xr:uid="{E77A8CF3-7C97-4AFC-928F-015B094346B0}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Space Optimization using Bit Manipulation
</commit_message>
<xml_diff>
--- a/DSA_sheet.xlsx
+++ b/DSA_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PKIRANMU\Desktop\DSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF14A604-BFE0-4D59-AED1-31622B98B582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED9235B-B0D0-4E62-A7EB-53F415039F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,10 +24,10 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
+    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 1" guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 3" guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 2" guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 4" guid="{8391B649-8505-4799-A195-AB43CB26E425}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1259" uniqueCount="701">
   <si>
     <t>DSA by Shradha Ma'am</t>
   </si>
@@ -2739,7 +2739,7 @@
   <dimension ref="A1:AC914"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScale="105" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3775,6 +3775,9 @@
         <v>54</v>
       </c>
       <c r="C28" s="11"/>
+      <c r="D28" s="40" t="s">
+        <v>700</v>
+      </c>
       <c r="E28" s="12" t="s">
         <v>55</v>
       </c>
@@ -3811,7 +3814,9 @@
         <v>56</v>
       </c>
       <c r="C29" s="11"/>
-      <c r="D29" s="41"/>
+      <c r="D29" s="40" t="s">
+        <v>700</v>
+      </c>
       <c r="E29" s="12" t="s">
         <v>53</v>
       </c>
@@ -33221,21 +33226,21 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:C37" xr:uid="{0ACB2A45-7D75-4140-937B-E1EEB2CA3B90}"/>
+      <autoFilter ref="A293:C332" xr:uid="{898F705B-02E1-4035-9DAF-28A2957768D4}"/>
+    </customSheetView>
+    <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A11:D37" xr:uid="{20DB233E-3794-4A76-8E31-12DBB885B708}"/>
     </customSheetView>
     <customSheetView guid="{1791E41F-2FB6-4B7D-BE94-80DC48681D60}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{5B33EC87-A986-47DA-AEE2-0FD74F8ADB55}"/>
+      <autoFilter ref="A11:D37" xr:uid="{854A1D4E-9F62-4B90-AE3B-02D1CCDB816A}"/>
     </customSheetView>
-    <customSheetView guid="{8391B649-8505-4799-A195-AB43CB26E425}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{64D3A7AF-0206-4BAD-A427-FE23D03476D4}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A11:D37" xr:uid="{5D3BF9DF-E222-4578-A829-977AD89160C5}"/>
-    </customSheetView>
-    <customSheetView guid="{AAC291DF-A190-44CD-BE51-531E90BAF94B}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332" xr:uid="{E77A8CF3-7C97-4AFC-928F-015B094346B0}"/>
+      <autoFilter ref="A11:C37" xr:uid="{81478CA2-2CCA-4B0B-B3F6-3C259D7E355A}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="1">

</xml_diff>